<commit_message>
added homework tasks and examples
</commit_message>
<xml_diff>
--- a/examen/eco-15-p-1.xlsx
+++ b/examen/eco-15-p-1.xlsx
@@ -109,7 +109,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -117,6 +117,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -423,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:AO14"/>
+  <dimension ref="B5:AP14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AR11" sqref="AR11"/>
+      <selection activeCell="AS10" sqref="AS10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,10 +437,12 @@
     <col min="2" max="2" width="6" customWidth="1"/>
     <col min="3" max="3" width="32.5703125" customWidth="1"/>
     <col min="4" max="37" width="10.7109375" hidden="1" customWidth="1"/>
-    <col min="40" max="40" width="7.28515625" customWidth="1"/>
+    <col min="38" max="38" width="11.140625" hidden="1" customWidth="1"/>
+    <col min="39" max="39" width="11.85546875" customWidth="1"/>
+    <col min="40" max="40" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
         <v>10</v>
@@ -533,31 +538,34 @@
         <v>43166</v>
       </c>
       <c r="AH5" s="3">
+        <v>43147</v>
+      </c>
+      <c r="AI5" s="3">
         <v>43154</v>
       </c>
-      <c r="AI5" s="3">
+      <c r="AJ5" s="3">
         <v>43153</v>
       </c>
-      <c r="AJ5" s="3">
+      <c r="AK5" s="3">
         <v>43152</v>
       </c>
-      <c r="AK5" s="3">
+      <c r="AL5" s="3">
         <v>43151</v>
       </c>
-      <c r="AL5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AM5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AN5" s="1" t="s">
+      <c r="AM5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AO5" s="1" t="s">
+      <c r="AP5" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>1</v>
       </c>
@@ -664,17 +672,23 @@
         <v>1</v>
       </c>
       <c r="AK6" s="2">
-        <v>11</v>
-      </c>
-      <c r="AL6" s="4">
-        <f>SUM(D6:AK6)/34</f>
-        <v>5.117647058823529</v>
-      </c>
-      <c r="AM6" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="AL6" s="2">
+        <v>11</v>
+      </c>
+      <c r="AM6" s="4">
+        <f>SUM(D6:AL6)/34</f>
+        <v>5.1470588235294121</v>
+      </c>
       <c r="AN6" s="1"/>
       <c r="AO6" s="1"/>
+      <c r="AP6" s="4">
+        <f t="shared" ref="AP6:AP14" si="0">60%*AM6+25%*AN6+15%*AO6</f>
+        <v>3.0882352941176472</v>
+      </c>
     </row>
-    <row r="7" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>2</v>
       </c>
@@ -783,15 +797,21 @@
       <c r="AK7" s="2">
         <v>1</v>
       </c>
-      <c r="AL7" s="4">
-        <f t="shared" ref="AL7:AL14" si="0">SUM(D7:AK7)/34</f>
-        <v>0.8529411764705882</v>
-      </c>
-      <c r="AM7" s="1"/>
+      <c r="AL7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AM7" s="4">
+        <f>SUM(D7:AL7)/34</f>
+        <v>0.88235294117647056</v>
+      </c>
       <c r="AN7" s="1"/>
       <c r="AO7" s="1"/>
+      <c r="AP7" s="4">
+        <f t="shared" si="0"/>
+        <v>0.52941176470588236</v>
+      </c>
     </row>
-    <row r="8" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>3</v>
       </c>
@@ -888,27 +908,33 @@
       <c r="AG8" s="2">
         <v>9</v>
       </c>
-      <c r="AH8" s="2">
+      <c r="AH8" s="5">
         <v>11</v>
       </c>
       <c r="AI8" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AJ8" s="2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AK8" s="2">
         <v>12</v>
       </c>
-      <c r="AL8" s="4">
-        <f t="shared" si="0"/>
-        <v>8.7941176470588243</v>
-      </c>
-      <c r="AM8" s="1"/>
+      <c r="AL8" s="2">
+        <v>12</v>
+      </c>
+      <c r="AM8" s="4">
+        <f>SUM(D8:AL8)/34</f>
+        <v>9.117647058823529</v>
+      </c>
       <c r="AN8" s="1"/>
       <c r="AO8" s="1"/>
+      <c r="AP8" s="4">
+        <f t="shared" si="0"/>
+        <v>5.4705882352941169</v>
+      </c>
     </row>
-    <row r="9" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>4</v>
       </c>
@@ -1015,17 +1041,23 @@
         <v>1</v>
       </c>
       <c r="AK9" s="2">
-        <v>10</v>
-      </c>
-      <c r="AL9" s="4">
-        <f t="shared" si="0"/>
-        <v>1.3235294117647058</v>
-      </c>
-      <c r="AM9" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="AL9" s="2">
+        <v>10</v>
+      </c>
+      <c r="AM9" s="4">
+        <f>SUM(D9:AL9)/34</f>
+        <v>1.3529411764705883</v>
+      </c>
       <c r="AN9" s="1"/>
       <c r="AO9" s="1"/>
+      <c r="AP9" s="4">
+        <f t="shared" si="0"/>
+        <v>0.81176470588235294</v>
+      </c>
     </row>
-    <row r="10" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>5</v>
       </c>
@@ -1122,27 +1154,33 @@
       <c r="AG10" s="2">
         <v>1</v>
       </c>
-      <c r="AH10" s="2">
-        <v>1</v>
+      <c r="AH10" s="5">
+        <v>11</v>
       </c>
       <c r="AI10" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AJ10" s="2">
+        <v>10</v>
+      </c>
+      <c r="AK10" s="2">
         <v>9</v>
       </c>
-      <c r="AK10" s="2">
-        <v>11</v>
-      </c>
-      <c r="AL10" s="4">
-        <f t="shared" si="0"/>
-        <v>8.117647058823529</v>
-      </c>
-      <c r="AM10" s="1"/>
+      <c r="AL10" s="2">
+        <v>11</v>
+      </c>
+      <c r="AM10" s="4">
+        <f>SUM(D10:AL10)/34</f>
+        <v>8.4411764705882355</v>
+      </c>
       <c r="AN10" s="1"/>
       <c r="AO10" s="1"/>
+      <c r="AP10" s="4">
+        <f t="shared" si="0"/>
+        <v>5.0647058823529409</v>
+      </c>
     </row>
-    <row r="11" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>6</v>
       </c>
@@ -1251,15 +1289,21 @@
       <c r="AK11" s="2">
         <v>1</v>
       </c>
-      <c r="AL11" s="4">
-        <f t="shared" si="0"/>
-        <v>0.8529411764705882</v>
-      </c>
-      <c r="AM11" s="1"/>
+      <c r="AL11" s="2">
+        <v>1</v>
+      </c>
+      <c r="AM11" s="4">
+        <f>SUM(D11:AL11)/34</f>
+        <v>0.88235294117647056</v>
+      </c>
       <c r="AN11" s="1"/>
       <c r="AO11" s="1"/>
+      <c r="AP11" s="4">
+        <f t="shared" si="0"/>
+        <v>0.52941176470588236</v>
+      </c>
     </row>
-    <row r="12" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>7</v>
       </c>
@@ -1356,7 +1400,7 @@
       <c r="AG12" s="2">
         <v>11</v>
       </c>
-      <c r="AH12" s="2">
+      <c r="AH12" s="5">
         <v>11</v>
       </c>
       <c r="AI12" s="2">
@@ -1368,15 +1412,21 @@
       <c r="AK12" s="2">
         <v>11</v>
       </c>
-      <c r="AL12" s="4">
-        <f t="shared" si="0"/>
-        <v>5.8235294117647056</v>
-      </c>
-      <c r="AM12" s="1"/>
+      <c r="AL12" s="2">
+        <v>11</v>
+      </c>
+      <c r="AM12" s="4">
+        <f>SUM(D12:AL12)/34</f>
+        <v>6.1470588235294121</v>
+      </c>
       <c r="AN12" s="1"/>
       <c r="AO12" s="1"/>
+      <c r="AP12" s="4">
+        <f t="shared" si="0"/>
+        <v>3.6882352941176473</v>
+      </c>
     </row>
-    <row r="13" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>8</v>
       </c>
@@ -1473,7 +1523,7 @@
       <c r="AG13" s="2">
         <v>12</v>
       </c>
-      <c r="AH13" s="2">
+      <c r="AH13" s="5">
         <v>12</v>
       </c>
       <c r="AI13" s="2">
@@ -1483,17 +1533,23 @@
         <v>12</v>
       </c>
       <c r="AK13" s="2">
-        <v>11</v>
-      </c>
-      <c r="AL13" s="4">
-        <f t="shared" si="0"/>
-        <v>10.764705882352942</v>
-      </c>
-      <c r="AM13" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="AL13" s="2">
+        <v>11</v>
+      </c>
+      <c r="AM13" s="4">
+        <f>SUM(D13:AL13)/34</f>
+        <v>11.117647058823529</v>
+      </c>
       <c r="AN13" s="1"/>
       <c r="AO13" s="1"/>
+      <c r="AP13" s="4">
+        <f t="shared" si="0"/>
+        <v>6.670588235294117</v>
+      </c>
     </row>
-    <row r="14" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>9</v>
       </c>
@@ -1600,18 +1656,36 @@
         <v>1</v>
       </c>
       <c r="AK14" s="2">
-        <v>11</v>
-      </c>
-      <c r="AL14" s="4">
-        <f t="shared" si="0"/>
-        <v>3.9117647058823528</v>
-      </c>
-      <c r="AM14" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="AL14" s="2">
+        <v>11</v>
+      </c>
+      <c r="AM14" s="4">
+        <f>SUM(D14:AL14)/34</f>
+        <v>3.9411764705882355</v>
+      </c>
       <c r="AN14" s="1"/>
       <c r="AO14" s="1"/>
+      <c r="AP14" s="4">
+        <f t="shared" si="0"/>
+        <v>2.3647058823529412</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="AL6:AL14">
+  <conditionalFormatting sqref="AM6:AM14">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AP6:AP14">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>